<commit_message>
latest version of data extraction files and added plots on direction of relationship
</commit_message>
<xml_diff>
--- a/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_Basurko.xlsx
+++ b/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_Basurko.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\use\Oihane_Cabezas\IM21_SEAWISE\Revision biblio WP4\Stage 2_papers\Instructions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://share.dtu.dk/sites/SEAwise_517900/Shared Documents/WP4 Ecological effects of fisheries/Task 4.1/Data extraction/Data extraction files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57277244-FF97-45F9-9004-27C0D55354F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3821678-5F0E-41E3-B176-ECC09AAEECB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataExtraction" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Drop-down overview" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DataExtraction!$A$2:$AX$48</definedName>
     <definedName name="Benthic_epifauna">Validation!$AI$32:$AI$35</definedName>
     <definedName name="Benthos">Validation!$AN$24:$AN$25</definedName>
     <definedName name="Catch_and_bycatch">Validation!$AM$15:$AM$17</definedName>
@@ -42,7 +43,7 @@
     <definedName name="Reptiles">Validation!$AM$24</definedName>
     <definedName name="Seines">Validation!$AS$31:$AS$35</definedName>
   </definedNames>
-  <calcPr calcId="191029" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -54,7 +55,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -2335,7 +2335,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2229" uniqueCount="642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2210" uniqueCount="636">
   <si>
     <t>SearchID</t>
   </si>
@@ -3902,15 +3902,6 @@
   </si>
   <si>
     <t>Relative and absolute growth _ linear regression _ modal progression _ software ELEFAN _ programme MIX _ mortality _ Yield per Recruit analysis _ sensitivity analysis _ Virtual population analysis (VPA) _ programme VIT _ programme MSFLA</t>
-  </si>
-  <si>
-    <t>Telephone survey and face-to-face interviews to anglers</t>
-  </si>
-  <si>
-    <t>Anglers motivation towards marine litter generation from angling</t>
-  </si>
-  <si>
-    <t>Considering the angling effort between 962,907 and 1,103,134 angling days distributed among different fishing platforms (boat, charter boat, shore) and a mean loss of 7.2 g lead per fishing day, the total deposition of lead by recreational anglers may be estimated to range between 6.9 and 7.9 t per year in German Baltic waters. The locally high number of marine anglers and angling effort indicates that angling related litter may be an environmental issue and should be considered in MRF and litter management.</t>
   </si>
   <si>
     <t>Phocoena phocoena</t>
@@ -4140,9 +4131,6 @@
     <t>Catch (in total number and weight per species caught)</t>
   </si>
   <si>
-    <t xml:space="preserve">Argentina sphyraena _ Arnoglossus laterna _ Arnoglossus thori _ Aspitrigla cuculus _ Belottia apoda _ Callionymus sp. _ Capros aper _ Cepola macrophthalma _ Citharus linguatula _ Conger conger _ Eutrigla gurnardus _ Gadiculus argenteus argenteus _ Gaidropsarus mediterraneus _ Galeus melastomus _ Gobiidae _ Gobius niger _ Lepidorhombus boscii _ Lepidotrigla cavillone _ Lophius budegassa _ Maurolicus muelleri _ Merluccius merluccius _ Microchirus variegatus _ Micromesistius poutassou _ Mullus barbatus _ Nephrops norvegicus _ Scyliorhinus canicula _ Serranus hepatus _ Solea vulgaris _ Symphurus ligulatus _ Torpedo marmorata _ Trachurus mediterraneus _ Trachurus trachurus _ Trigla lucerna _ Trigla lyra _ Trigloporus lastoviza _ Trisopterus minutus capelanus_ </t>
-  </si>
-  <si>
     <t>Argentina sphyraena _ Arnoglossus laterna _ Arnoglossus thori _ Aspitrigla cuculus _ Belottia apoda _ Callionymus sp. _ Capros aper _ Cepola macrophthalma _ Citharus linguatula _ Conger conger _ Eutrigla gurnardus _ Gadiculus argenteus argenteus _ Gaidropsarus mediterraneus _ Galeus melastomus _ Gobiidae _ Gobius niger _ Lepidorhombus boscii _ Lepidotrigla cavillone _ Lophius budegassa _ Maurolicus muelleri _ Merluccius merluccius _ Microchirus variegatus _ Micromesistius poutassou _ Mullus barbatus _ Nephrops norvegicus _ Scyliorhinus canicula _ Serranus hepatus _ Solea vulgaris _ Symphurus ligulatus _ Torpedo marmorata _ Trachurus mediterraneus _ Trachurus trachurus _ Trigla lucerna _ Trigla lyra _ Trigloporus lastoviza _ Trisopterus minutus capelanus _ Zeus faber</t>
   </si>
   <si>
@@ -4226,9 +4214,6 @@
     <t>Yiel for recruit (Y/R)</t>
   </si>
   <si>
-    <t>Release of marine litter into the environment</t>
-  </si>
-  <si>
     <t xml:space="preserve">Squalus acanthias _ Psetta maxima _ Trigla lucerna _ Raja clavata _ Phocoena phocoena </t>
   </si>
   <si>
@@ -4263,9 +4248,6 @@
   </si>
   <si>
     <t xml:space="preserve">Stomach fullness (%BW) _ mean partial fullness index for prey (PFIi) _ Chi-square test _ Mann–Whitney U-test _ Kruskal-Wallis non-parametric test </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Angler motivation _ EFA _ Tucker-Lewis Index _ root mean square residuals and root mean square error of approximation _ Multivariate fuzzy cluster analysis _ Spearman correlation _ Kruskal-Wallis non-parametric test  _ Dunn's post hoc test _  Poisson regression _ Chi-square test _ R _ </t>
   </si>
 </sst>
 </file>
@@ -4882,13 +4864,13 @@
   <dimension ref="A1:AX49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="T3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="X36" sqref="X36"/>
+      <selection pane="bottomRight" activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="13" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="5" customWidth="1"/>
     <col min="3" max="3" width="24.5546875" customWidth="1"/>
@@ -5308,7 +5290,7 @@
         <v>485</v>
       </c>
       <c r="Z4" s="37" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="AA4" s="37">
         <v>2</v>
@@ -5340,14 +5322,14 @@
       </c>
       <c r="AK4" s="37"/>
       <c r="AL4" s="37" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="AM4" s="37" t="s">
         <v>233</v>
       </c>
       <c r="AN4" s="37"/>
       <c r="AO4" s="37" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="AP4" s="37"/>
       <c r="AQ4" s="37" t="s">
@@ -5361,7 +5343,7 @@
       </c>
       <c r="AT4" s="37"/>
       <c r="AU4" s="37" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="AV4" s="37" t="s">
         <v>214</v>
@@ -5370,7 +5352,7 @@
         <v>211</v>
       </c>
       <c r="AX4" s="37" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="5" spans="1:50" s="15" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -5448,7 +5430,7 @@
         <v>486</v>
       </c>
       <c r="Z5" s="40" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="AA5" s="40">
         <v>2</v>
@@ -5461,7 +5443,7 @@
       </c>
       <c r="AD5" s="40"/>
       <c r="AE5" s="40" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="AF5" s="40" t="s">
         <v>280</v>
@@ -5480,17 +5462,17 @@
       </c>
       <c r="AK5" s="40"/>
       <c r="AL5" s="40" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="AM5" s="40" t="s">
         <v>234</v>
       </c>
       <c r="AN5" s="40"/>
       <c r="AO5" s="40" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="AP5" s="40" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="AQ5" s="40" t="s">
         <v>166</v>
@@ -5503,7 +5485,7 @@
       </c>
       <c r="AT5" s="40"/>
       <c r="AU5" s="40" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="AV5" s="40" t="s">
         <v>240</v>
@@ -5512,7 +5494,7 @@
         <v>210</v>
       </c>
       <c r="AX5" s="40" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="6" spans="1:50" s="15" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -5590,7 +5572,7 @@
         <v>486</v>
       </c>
       <c r="Z6" s="23" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="AA6" s="23">
         <v>2</v>
@@ -5603,7 +5585,7 @@
       </c>
       <c r="AD6" s="23"/>
       <c r="AE6" s="23" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="AF6" s="23" t="s">
         <v>280</v>
@@ -5622,17 +5604,17 @@
       </c>
       <c r="AK6" s="23"/>
       <c r="AL6" s="23" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="AM6" s="23" t="s">
         <v>234</v>
       </c>
       <c r="AN6" s="23"/>
       <c r="AO6" s="23" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="AP6" s="23" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="AQ6" s="23" t="s">
         <v>166</v>
@@ -5645,7 +5627,7 @@
       </c>
       <c r="AT6" s="23"/>
       <c r="AU6" s="23" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="AV6" s="23" t="s">
         <v>206</v>
@@ -5654,7 +5636,7 @@
         <v>210</v>
       </c>
       <c r="AX6" s="23" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="7" spans="1:50" s="15" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -5732,7 +5714,7 @@
         <v>486</v>
       </c>
       <c r="Z7" s="23" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="AA7" s="23">
         <v>2</v>
@@ -5745,7 +5727,7 @@
       </c>
       <c r="AD7" s="23"/>
       <c r="AE7" s="23" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="AF7" s="23" t="s">
         <v>280</v>
@@ -5764,17 +5746,17 @@
       </c>
       <c r="AK7" s="23"/>
       <c r="AL7" s="23" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="AM7" s="23" t="s">
         <v>234</v>
       </c>
       <c r="AN7" s="23"/>
       <c r="AO7" s="23" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="AP7" s="23" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="AQ7" s="23" t="s">
         <v>166</v>
@@ -5786,10 +5768,10 @@
         <v>192</v>
       </c>
       <c r="AT7" s="23" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="AU7" s="23" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="AV7" s="23" t="s">
         <v>115</v>
@@ -5798,7 +5780,7 @@
         <v>212</v>
       </c>
       <c r="AX7" s="23" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
     </row>
     <row r="8" spans="1:50" s="16" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -5873,10 +5855,10 @@
         <v>75</v>
       </c>
       <c r="Y8" s="40" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="Z8" s="40" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="AA8" s="43">
         <v>2</v>
@@ -5904,14 +5886,14 @@
       <c r="AJ8" s="43"/>
       <c r="AK8" s="43"/>
       <c r="AL8" s="43" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="AM8" s="43" t="s">
         <v>235</v>
       </c>
       <c r="AN8" s="43"/>
       <c r="AO8" s="43" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="AP8" s="43"/>
       <c r="AQ8" s="43" t="s">
@@ -5924,10 +5906,10 @@
         <v>177</v>
       </c>
       <c r="AT8" s="43" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="AU8" s="43" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="AV8" s="43" t="s">
         <v>201</v>
@@ -5936,7 +5918,7 @@
         <v>210</v>
       </c>
       <c r="AX8" s="40" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="9" spans="1:50" s="16" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -6011,10 +5993,10 @@
         <v>75</v>
       </c>
       <c r="Y9" s="23" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="Z9" s="23" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="AA9" s="26">
         <v>2</v>
@@ -6042,14 +6024,14 @@
       <c r="AJ9" s="26"/>
       <c r="AK9" s="26"/>
       <c r="AL9" s="26" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="AM9" s="26" t="s">
         <v>235</v>
       </c>
       <c r="AN9" s="26"/>
       <c r="AO9" s="26" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="AP9" s="26"/>
       <c r="AQ9" s="26" t="s">
@@ -6062,10 +6044,10 @@
         <v>177</v>
       </c>
       <c r="AT9" s="26" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="AU9" s="26" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="AV9" s="26" t="s">
         <v>115</v>
@@ -6074,7 +6056,7 @@
         <v>212</v>
       </c>
       <c r="AX9" s="23" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
     <row r="10" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -6242,7 +6224,7 @@
         <v>487</v>
       </c>
       <c r="Z11" s="40" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
       <c r="AA11" s="43">
         <v>2</v>
@@ -6277,10 +6259,10 @@
       </c>
       <c r="AN11" s="43"/>
       <c r="AO11" s="43" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="AP11" s="43" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="AQ11" s="43" t="s">
         <v>166</v>
@@ -6304,7 +6286,7 @@
         <v>210</v>
       </c>
       <c r="AX11" s="40" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
     </row>
     <row r="12" spans="1:50" s="17" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -6382,7 +6364,7 @@
         <v>487</v>
       </c>
       <c r="Z12" s="23" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
       <c r="AA12" s="26">
         <v>2</v>
@@ -6417,10 +6399,10 @@
       </c>
       <c r="AN12" s="26"/>
       <c r="AO12" s="26" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="AP12" s="26" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="AQ12" s="26" t="s">
         <v>166</v>
@@ -6435,7 +6417,7 @@
         <v>490</v>
       </c>
       <c r="AU12" s="26" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="AV12" s="26" t="s">
         <v>201</v>
@@ -6444,7 +6426,7 @@
         <v>210</v>
       </c>
       <c r="AX12" s="23" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
     </row>
     <row r="13" spans="1:50" s="16" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6518,7 +6500,7 @@
         <v>492</v>
       </c>
       <c r="Z13" s="40" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="AA13" s="43">
         <v>2</v>
@@ -6552,7 +6534,7 @@
         <v>136</v>
       </c>
       <c r="AL13" s="43" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="AM13" s="43" t="s">
         <v>234</v>
@@ -6575,7 +6557,7 @@
       </c>
       <c r="AT13" s="40"/>
       <c r="AU13" s="40" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="AV13" s="43" t="s">
         <v>215</v>
@@ -6584,7 +6566,7 @@
         <v>210</v>
       </c>
       <c r="AX13" s="40" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
     </row>
     <row r="14" spans="1:50" s="16" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6658,7 +6640,7 @@
         <v>492</v>
       </c>
       <c r="Z14" s="23" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="AA14" s="26">
         <v>2</v>
@@ -6692,7 +6674,7 @@
         <v>136</v>
       </c>
       <c r="AL14" s="26" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="AM14" s="26" t="s">
         <v>234</v>
@@ -6715,7 +6697,7 @@
       </c>
       <c r="AT14" s="23"/>
       <c r="AU14" s="23" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="AV14" s="26" t="s">
         <v>201</v>
@@ -6724,7 +6706,7 @@
         <v>210</v>
       </c>
       <c r="AX14" s="23" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
     </row>
     <row r="15" spans="1:50" s="16" customFormat="1" x14ac:dyDescent="0.3">
@@ -6982,7 +6964,7 @@
       </c>
       <c r="Y17" s="46"/>
       <c r="Z17" s="46" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="AA17" s="46">
         <v>2</v>
@@ -7029,7 +7011,7 @@
       </c>
       <c r="AT17" s="46"/>
       <c r="AU17" s="46" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="AV17" s="46" t="s">
         <v>201</v>
@@ -7241,10 +7223,10 @@
         <v>162</v>
       </c>
       <c r="AO19" s="54" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="AP19" s="54" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="AQ19" s="54" t="s">
         <v>166</v>
@@ -7259,7 +7241,7 @@
         <v>499</v>
       </c>
       <c r="AU19" s="54" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="AV19" s="54" t="s">
         <v>201</v>
@@ -7397,7 +7379,7 @@
         <v>499</v>
       </c>
       <c r="AU20" s="28" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="AV20" s="28" t="s">
         <v>201</v>
@@ -7484,7 +7466,7 @@
         <v>506</v>
       </c>
       <c r="Z21" s="54" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="AA21" s="54">
         <v>1</v>
@@ -7514,14 +7496,14 @@
       <c r="AJ21" s="54"/>
       <c r="AK21" s="54"/>
       <c r="AL21" s="54" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="AM21" s="54" t="s">
         <v>161</v>
       </c>
       <c r="AN21" s="54"/>
       <c r="AO21" s="54" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="AP21" s="54"/>
       <c r="AQ21" s="54" t="s">
@@ -7534,10 +7516,10 @@
         <v>177</v>
       </c>
       <c r="AT21" s="54" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="AU21" s="54" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="AV21" s="54" t="s">
         <v>205</v>
@@ -7546,7 +7528,7 @@
         <v>209</v>
       </c>
       <c r="AX21" s="54" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="22" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -7624,7 +7606,7 @@
         <v>506</v>
       </c>
       <c r="Z22" s="28" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="AA22" s="28">
         <v>1</v>
@@ -7654,14 +7636,14 @@
       <c r="AJ22" s="28"/>
       <c r="AK22" s="28"/>
       <c r="AL22" s="28" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="AM22" s="28" t="s">
         <v>234</v>
       </c>
       <c r="AN22" s="28"/>
       <c r="AO22" s="28" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="AP22" s="28"/>
       <c r="AQ22" s="28" t="s">
@@ -7674,10 +7656,10 @@
         <v>177</v>
       </c>
       <c r="AT22" s="28" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="AU22" s="28" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="AV22" s="28" t="s">
         <v>208</v>
@@ -7686,7 +7668,7 @@
         <v>209</v>
       </c>
       <c r="AX22" s="28" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="23" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -7854,7 +7836,7 @@
         <v>506</v>
       </c>
       <c r="Z24" s="54" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="AA24" s="54">
         <v>2</v>
@@ -7884,14 +7866,14 @@
       <c r="AJ24" s="54"/>
       <c r="AK24" s="54"/>
       <c r="AL24" s="54" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="AM24" s="54" t="s">
         <v>235</v>
       </c>
       <c r="AN24" s="54"/>
       <c r="AO24" s="54" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="AP24" s="54"/>
       <c r="AQ24" s="54" t="s">
@@ -7907,7 +7889,7 @@
         <v>501</v>
       </c>
       <c r="AU24" s="54" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="AV24" s="54" t="s">
         <v>205</v>
@@ -7916,7 +7898,7 @@
         <v>209</v>
       </c>
       <c r="AX24" s="54" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="25" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -7994,7 +7976,7 @@
         <v>506</v>
       </c>
       <c r="Z25" s="28" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="AA25" s="28">
         <v>2</v>
@@ -8024,7 +8006,7 @@
       <c r="AJ25" s="28"/>
       <c r="AK25" s="28"/>
       <c r="AL25" s="28" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="AM25" s="28" t="s">
         <v>234</v>
@@ -8033,7 +8015,7 @@
         <v>162</v>
       </c>
       <c r="AO25" s="28" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="AP25" s="28"/>
       <c r="AQ25" s="28" t="s">
@@ -8049,7 +8031,7 @@
         <v>501</v>
       </c>
       <c r="AU25" s="28" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="AV25" s="28" t="s">
         <v>205</v>
@@ -8058,7 +8040,7 @@
         <v>212</v>
       </c>
       <c r="AX25" s="28" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
     </row>
     <row r="26" spans="1:50" s="16" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -8134,7 +8116,7 @@
       </c>
       <c r="Y26" s="43"/>
       <c r="Z26" s="43" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="AA26" s="43">
         <v>2</v>
@@ -8167,10 +8149,10 @@
       </c>
       <c r="AN26" s="43"/>
       <c r="AO26" s="43" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="AP26" s="43" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="AQ26" s="43" t="s">
         <v>166</v>
@@ -8182,7 +8164,7 @@
         <v>178</v>
       </c>
       <c r="AT26" s="43" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="AU26" s="43" t="s">
         <v>495</v>
@@ -8194,7 +8176,7 @@
         <v>210</v>
       </c>
       <c r="AX26" s="40" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
     </row>
     <row r="27" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -8270,7 +8252,7 @@
       </c>
       <c r="Y27" s="54"/>
       <c r="Z27" s="54" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
       <c r="AA27" s="54">
         <v>2</v>
@@ -8309,7 +8291,7 @@
         <v>162</v>
       </c>
       <c r="AO27" s="54" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="AP27" s="54"/>
       <c r="AQ27" s="54" t="s">
@@ -8323,7 +8305,7 @@
         <v>503</v>
       </c>
       <c r="AU27" s="54" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="AV27" s="54" t="s">
         <v>201</v>
@@ -8332,7 +8314,7 @@
         <v>210</v>
       </c>
       <c r="AX27" s="54" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
     </row>
     <row r="28" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -8410,7 +8392,7 @@
         <v>507</v>
       </c>
       <c r="Z28" s="54" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
       <c r="AA28" s="54">
         <v>2</v>
@@ -8442,14 +8424,14 @@
         <v>143</v>
       </c>
       <c r="AL28" s="54" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="AM28" s="54" t="s">
         <v>235</v>
       </c>
       <c r="AN28" s="54"/>
       <c r="AO28" s="54" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="AP28" s="54"/>
       <c r="AQ28" s="54" t="s">
@@ -8460,10 +8442,10 @@
       </c>
       <c r="AS28" s="54"/>
       <c r="AT28" s="54" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="AU28" s="54" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="AV28" s="54" t="s">
         <v>201</v>
@@ -8472,7 +8454,7 @@
         <v>210</v>
       </c>
       <c r="AX28" s="54" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
     </row>
     <row r="29" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -8550,7 +8532,7 @@
         <v>507</v>
       </c>
       <c r="Z29" s="28" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
       <c r="AA29" s="28">
         <v>2</v>
@@ -8582,14 +8564,14 @@
         <v>143</v>
       </c>
       <c r="AL29" s="28" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="AM29" s="28" t="s">
         <v>235</v>
       </c>
       <c r="AN29" s="28"/>
       <c r="AO29" s="28" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="AP29" s="28"/>
       <c r="AQ29" s="28" t="s">
@@ -8600,10 +8582,10 @@
       </c>
       <c r="AS29" s="28"/>
       <c r="AT29" s="28" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="AU29" s="28" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="AV29" s="28" t="s">
         <v>201</v>
@@ -8612,7 +8594,7 @@
         <v>210</v>
       </c>
       <c r="AX29" s="28" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
     </row>
     <row r="30" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -8780,7 +8762,7 @@
         <v>509</v>
       </c>
       <c r="Z31" s="54" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="AA31" s="54">
         <v>2</v>
@@ -8810,7 +8792,7 @@
       <c r="AJ31" s="54"/>
       <c r="AK31" s="54"/>
       <c r="AL31" s="54" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="AM31" s="54" t="s">
         <v>234</v>
@@ -8819,10 +8801,10 @@
         <v>162</v>
       </c>
       <c r="AO31" s="54" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="AP31" s="54" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="AQ31" s="54" t="s">
         <v>166</v>
@@ -8834,7 +8816,7 @@
         <v>183</v>
       </c>
       <c r="AT31" s="54" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="AU31" s="54" t="s">
         <v>510</v>
@@ -8924,7 +8906,7 @@
         <v>509</v>
       </c>
       <c r="Z32" s="28" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="AA32" s="28">
         <v>2</v>
@@ -8954,7 +8936,7 @@
       <c r="AJ32" s="28"/>
       <c r="AK32" s="28"/>
       <c r="AL32" s="28" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="AM32" s="28" t="s">
         <v>234</v>
@@ -8963,10 +8945,10 @@
         <v>162</v>
       </c>
       <c r="AO32" s="28" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="AP32" s="28" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="AQ32" s="28" t="s">
         <v>166</v>
@@ -8978,10 +8960,10 @@
         <v>183</v>
       </c>
       <c r="AT32" s="28" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="AU32" s="28" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="AV32" s="28" t="s">
         <v>201</v>
@@ -9105,7 +9087,7 @@
         <v>162</v>
       </c>
       <c r="AO33" s="54" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="AP33" s="54"/>
       <c r="AQ33" s="54" t="s">
@@ -9118,10 +9100,10 @@
         <v>178</v>
       </c>
       <c r="AT33" s="54" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="AU33" s="54" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="AV33" s="54" t="s">
         <v>201</v>
@@ -9130,7 +9112,7 @@
         <v>211</v>
       </c>
       <c r="AX33" s="55" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
     </row>
     <row r="34" spans="1:50" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -9245,7 +9227,7 @@
         <v>162</v>
       </c>
       <c r="AO34" s="28" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="AP34" s="28"/>
       <c r="AQ34" s="28" t="s">
@@ -9258,10 +9240,10 @@
         <v>178</v>
       </c>
       <c r="AT34" s="28" t="s">
+        <v>597</v>
+      </c>
+      <c r="AU34" s="28" t="s">
         <v>601</v>
-      </c>
-      <c r="AU34" s="28" t="s">
-        <v>605</v>
       </c>
       <c r="AV34" s="28" t="s">
         <v>201</v>
@@ -9270,7 +9252,7 @@
         <v>210</v>
       </c>
       <c r="AX34" s="31" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="35" spans="1:50" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -9385,7 +9367,7 @@
         <v>162</v>
       </c>
       <c r="AO35" s="28" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="AP35" s="28"/>
       <c r="AQ35" s="28" t="s">
@@ -9398,10 +9380,10 @@
         <v>178</v>
       </c>
       <c r="AT35" s="28" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="AU35" s="28" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="AV35" s="28" t="s">
         <v>201</v>
@@ -9410,7 +9392,7 @@
         <v>210</v>
       </c>
       <c r="AX35" s="31" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
     </row>
     <row r="36" spans="1:50" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -9525,7 +9507,7 @@
         <v>162</v>
       </c>
       <c r="AO36" s="28" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="AP36" s="28"/>
       <c r="AQ36" s="28" t="s">
@@ -9538,10 +9520,10 @@
         <v>178</v>
       </c>
       <c r="AT36" s="28" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="AU36" s="28" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="AV36" s="28" t="s">
         <v>201</v>
@@ -9550,7 +9532,7 @@
         <v>209</v>
       </c>
       <c r="AX36" s="31" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
     </row>
     <row r="37" spans="1:50" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -9665,7 +9647,7 @@
         <v>162</v>
       </c>
       <c r="AO37" s="28" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="AP37" s="28"/>
       <c r="AQ37" s="28" t="s">
@@ -9678,10 +9660,10 @@
         <v>178</v>
       </c>
       <c r="AT37" s="28" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="AU37" s="28" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="AV37" s="28" t="s">
         <v>201</v>
@@ -9690,7 +9672,7 @@
         <v>212</v>
       </c>
       <c r="AX37" s="31" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
     </row>
     <row r="38" spans="1:50" s="10" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -9768,7 +9750,7 @@
         <v>517</v>
       </c>
       <c r="Z38" s="54" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
       <c r="AA38" s="54">
         <v>2</v>
@@ -9803,7 +9785,7 @@
       </c>
       <c r="AN38" s="54"/>
       <c r="AO38" s="54" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="AP38" s="54"/>
       <c r="AQ38" s="54" t="s">
@@ -9819,7 +9801,7 @@
         <v>515</v>
       </c>
       <c r="AU38" s="54" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="AV38" s="54" t="s">
         <v>201</v>
@@ -9828,7 +9810,7 @@
         <v>210</v>
       </c>
       <c r="AX38" s="55" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
     </row>
     <row r="39" spans="1:50" s="10" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -9906,7 +9888,7 @@
         <v>517</v>
       </c>
       <c r="Z39" s="28" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
       <c r="AA39" s="28">
         <v>2</v>
@@ -9941,7 +9923,7 @@
       </c>
       <c r="AN39" s="28"/>
       <c r="AO39" s="28" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="AP39" s="28"/>
       <c r="AQ39" s="28" t="s">
@@ -9957,7 +9939,7 @@
         <v>515</v>
       </c>
       <c r="AU39" s="28" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="AV39" s="28" t="s">
         <v>201</v>
@@ -9966,7 +9948,7 @@
         <v>210</v>
       </c>
       <c r="AX39" s="31" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
     </row>
     <row r="40" spans="1:50" s="10" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -10044,7 +10026,7 @@
         <v>517</v>
       </c>
       <c r="Z40" s="28" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
       <c r="AA40" s="28">
         <v>2</v>
@@ -10079,7 +10061,7 @@
       </c>
       <c r="AN40" s="28"/>
       <c r="AO40" s="28" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="AP40" s="28"/>
       <c r="AQ40" s="28" t="s">
@@ -10095,7 +10077,7 @@
         <v>515</v>
       </c>
       <c r="AU40" s="28" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="AV40" s="28" t="s">
         <v>201</v>
@@ -10104,7 +10086,7 @@
         <v>209</v>
       </c>
       <c r="AX40" s="31" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
     </row>
     <row r="41" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -10182,7 +10164,7 @@
         <v>518</v>
       </c>
       <c r="Z41" s="54" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
       <c r="AA41" s="54">
         <v>2</v>
@@ -10217,7 +10199,7 @@
       </c>
       <c r="AN41" s="54"/>
       <c r="AO41" s="54" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="AP41" s="54"/>
       <c r="AQ41" s="54" t="s">
@@ -10230,10 +10212,10 @@
         <v>177</v>
       </c>
       <c r="AT41" s="54" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="AU41" s="54" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="AV41" s="54" t="s">
         <v>205</v>
@@ -10242,7 +10224,7 @@
         <v>209</v>
       </c>
       <c r="AX41" s="54" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="42" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -10320,7 +10302,7 @@
         <v>518</v>
       </c>
       <c r="Z42" s="28" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
       <c r="AA42" s="28">
         <v>2</v>
@@ -10355,7 +10337,7 @@
       </c>
       <c r="AN42" s="28"/>
       <c r="AO42" s="28" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="AP42" s="28"/>
       <c r="AQ42" s="28" t="s">
@@ -10368,10 +10350,10 @@
         <v>177</v>
       </c>
       <c r="AT42" s="28" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="AU42" s="28" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="AV42" s="28" t="s">
         <v>205</v>
@@ -10380,7 +10362,7 @@
         <v>209</v>
       </c>
       <c r="AX42" s="28" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="43" spans="1:50" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -10491,7 +10473,7 @@
         <v>162</v>
       </c>
       <c r="AO43" s="54" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="AP43" s="54"/>
       <c r="AQ43" s="54" t="s">
@@ -10507,7 +10489,7 @@
         <v>520</v>
       </c>
       <c r="AU43" s="54" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="AV43" s="54" t="s">
         <v>206</v>
@@ -10516,7 +10498,7 @@
         <v>209</v>
       </c>
       <c r="AX43" s="54" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="44" spans="1:50" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -10627,7 +10609,7 @@
         <v>162</v>
       </c>
       <c r="AO44" s="28" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="AP44" s="28"/>
       <c r="AQ44" s="28" t="s">
@@ -10643,7 +10625,7 @@
         <v>520</v>
       </c>
       <c r="AU44" s="28" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="AV44" s="28" t="s">
         <v>206</v>
@@ -10652,7 +10634,7 @@
         <v>209</v>
       </c>
       <c r="AX44" s="28" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="45" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -10763,7 +10745,7 @@
         <v>162</v>
       </c>
       <c r="AO45" s="28" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="AP45" s="28"/>
       <c r="AQ45" s="28" t="s">
@@ -10779,7 +10761,7 @@
         <v>520</v>
       </c>
       <c r="AU45" s="28" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="AV45" s="28" t="s">
         <v>206</v>
@@ -10788,7 +10770,7 @@
         <v>209</v>
       </c>
       <c r="AX45" s="28" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="46" spans="1:50" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -10925,85 +10907,41 @@
       <c r="Q47" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="R47" s="58"/>
-      <c r="S47" s="58" t="s">
-        <v>23</v>
-      </c>
-      <c r="T47" s="58" t="s">
-        <v>46</v>
-      </c>
-      <c r="U47" s="58" t="s">
-        <v>52</v>
-      </c>
-      <c r="V47" s="58" t="s">
-        <v>42</v>
-      </c>
-      <c r="W47" s="58" t="s">
-        <v>47</v>
-      </c>
-      <c r="X47" s="58" t="s">
-        <v>115</v>
-      </c>
-      <c r="Y47" s="58" t="s">
-        <v>522</v>
-      </c>
-      <c r="Z47" s="58" t="s">
-        <v>641</v>
-      </c>
-      <c r="AA47" s="58">
-        <v>2</v>
-      </c>
-      <c r="AB47" s="58">
-        <v>2</v>
-      </c>
-      <c r="AC47" s="58">
-        <v>3</v>
-      </c>
+      <c r="R47" s="58" t="s">
+        <v>84</v>
+      </c>
+      <c r="S47" s="58"/>
+      <c r="T47" s="58"/>
+      <c r="U47" s="58"/>
+      <c r="V47" s="58"/>
+      <c r="W47" s="58"/>
+      <c r="X47" s="58"/>
+      <c r="Y47" s="58"/>
+      <c r="Z47" s="58"/>
+      <c r="AA47" s="58"/>
+      <c r="AB47" s="58"/>
+      <c r="AC47" s="58"/>
       <c r="AD47" s="58"/>
       <c r="AE47" s="58"/>
-      <c r="AF47" s="58" t="s">
-        <v>269</v>
-      </c>
-      <c r="AG47" s="58" t="s">
-        <v>115</v>
-      </c>
+      <c r="AF47" s="58"/>
+      <c r="AG47" s="58"/>
       <c r="AH47" s="58"/>
       <c r="AI47" s="58"/>
       <c r="AJ47" s="58"/>
       <c r="AK47" s="58"/>
       <c r="AL47" s="58"/>
-      <c r="AM47" s="58" t="s">
-        <v>233</v>
-      </c>
+      <c r="AM47" s="58"/>
       <c r="AN47" s="58"/>
-      <c r="AO47" s="58" t="s">
-        <v>523</v>
-      </c>
+      <c r="AO47" s="58"/>
       <c r="AP47" s="58"/>
-      <c r="AQ47" s="58" t="s">
-        <v>167</v>
-      </c>
-      <c r="AR47" s="58" t="s">
-        <v>199</v>
-      </c>
-      <c r="AS47" s="58" t="s">
-        <v>198</v>
-      </c>
-      <c r="AT47" s="58" t="s">
-        <v>600</v>
-      </c>
-      <c r="AU47" s="58" t="s">
-        <v>628</v>
-      </c>
-      <c r="AV47" s="58" t="s">
-        <v>214</v>
-      </c>
-      <c r="AW47" s="58" t="s">
-        <v>209</v>
-      </c>
-      <c r="AX47" s="58" t="s">
-        <v>524</v>
-      </c>
+      <c r="AQ47" s="58"/>
+      <c r="AR47" s="58"/>
+      <c r="AS47" s="58"/>
+      <c r="AT47" s="58"/>
+      <c r="AU47" s="58"/>
+      <c r="AV47" s="58"/>
+      <c r="AW47" s="58"/>
+      <c r="AX47" s="58"/>
     </row>
     <row r="48" spans="1:50" s="16" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="41" t="s">
@@ -11071,10 +11009,10 @@
         <v>69</v>
       </c>
       <c r="Y48" s="43" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="Z48" s="43" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="AA48" s="43">
         <v>2</v>
@@ -11104,7 +11042,7 @@
       </c>
       <c r="AK48" s="43"/>
       <c r="AL48" s="43" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="AM48" s="43" t="s">
         <v>234</v>
@@ -11113,7 +11051,7 @@
         <v>164</v>
       </c>
       <c r="AO48" s="43" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="AP48" s="43"/>
       <c r="AQ48" s="43" t="s">
@@ -11126,10 +11064,10 @@
         <v>190</v>
       </c>
       <c r="AT48" s="43" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="AU48" s="43" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="AV48" s="43" t="s">
         <v>214</v>
@@ -11138,7 +11076,7 @@
         <v>212</v>
       </c>
       <c r="AX48" s="43" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
     <row r="49" spans="1:50" x14ac:dyDescent="0.3">
@@ -11326,7 +11264,7 @@
       <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="18" max="18" width="24.44140625" customWidth="1"/>
     <col min="19" max="19" width="32.109375" customWidth="1"/>
@@ -12399,7 +12337,7 @@
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
@@ -13273,12 +13211,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13396,15 +13331,25 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66D459FE-C8DA-484C-BC8E-5EB6A351EBC9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -13426,16 +13371,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66D459FE-C8DA-484C-BC8E-5EB6A351EBC9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>